<commit_message>
Test that poolname can be non-numeric
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1604.8.rml.xlsx
+++ b/tests/fixtures/orderforms/1604.8.rml.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FE698C-C06A-254C-8E1E-36BBAD8ABD9B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1318F94-542E-0743-A8E3-BB506A21ADDA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16840" yWindow="14180" windowWidth="32460" windowHeight="15340" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10000" yWindow="6820" windowWidth="32460" windowHeight="15340" tabRatio="211" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order form" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Index" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4897" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4899" uniqueCount="1237">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -3735,6 +3738,9 @@
   </si>
   <si>
     <t>AL-P-00110148-N-03127604-TP20170817-CB20170822</t>
+  </si>
+  <si>
+    <t>pool-1</t>
   </si>
 </sst>
 </file>
@@ -4951,15 +4957,6 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="44" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
@@ -5003,6 +5000,15 @@
     <xf numFmtId="0" fontId="47" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="241">
@@ -5378,6 +5384,21 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Index"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5684,7 +5705,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5728,7 +5749,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -5756,7 +5777,7 @@
   <dimension ref="A1:AA405"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13"/>
@@ -6182,23 +6203,23 @@
       <c r="AA14" s="6"/>
     </row>
     <row r="15" spans="1:27" s="7" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="171" t="s">
+      <c r="A15" s="182" t="s">
         <v>518</v>
       </c>
-      <c r="B15" s="172"/>
-      <c r="C15" s="172"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="172"/>
-      <c r="I15" s="172"/>
-      <c r="J15" s="173"/>
+      <c r="B15" s="183"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="183"/>
+      <c r="E15" s="183"/>
+      <c r="F15" s="183"/>
+      <c r="G15" s="183"/>
+      <c r="H15" s="183"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="184"/>
       <c r="K15" s="62"/>
-      <c r="L15" s="171" t="s">
+      <c r="L15" s="182" t="s">
         <v>522</v>
       </c>
-      <c r="M15" s="173"/>
+      <c r="M15" s="184"/>
       <c r="N15" s="62"/>
       <c r="O15" s="36" t="s">
         <v>88</v>
@@ -6208,10 +6229,10 @@
         <v>519</v>
       </c>
       <c r="R15" s="62"/>
-      <c r="S15" s="171" t="s">
+      <c r="S15" s="182" t="s">
         <v>520</v>
       </c>
-      <c r="T15" s="173"/>
+      <c r="T15" s="184"/>
       <c r="U15" s="18"/>
       <c r="V15" s="30"/>
       <c r="W15" s="30"/>
@@ -6444,41 +6465,41 @@
       <c r="AA20" s="12"/>
     </row>
     <row r="21" spans="1:27" s="113" customFormat="1" ht="25" customHeight="1">
-      <c r="A21" s="174" t="s">
+      <c r="A21" s="171" t="s">
         <v>1232</v>
       </c>
-      <c r="B21" s="175">
+      <c r="B21" s="172" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C21" s="173" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="174" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="175" t="s">
+        <v>1233</v>
+      </c>
+      <c r="F21" s="176" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="176">
+        <v>30</v>
+      </c>
+      <c r="H21" s="177">
+        <v>5</v>
+      </c>
+      <c r="I21" s="177" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="177">
         <v>1</v>
       </c>
-      <c r="C21" s="176" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="177" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="178" t="s">
-        <v>1233</v>
-      </c>
-      <c r="F21" s="179" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="179">
-        <v>30</v>
-      </c>
-      <c r="H21" s="180">
-        <v>5</v>
-      </c>
-      <c r="I21" s="180" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" s="180">
-        <v>1</v>
-      </c>
       <c r="K21" s="107"/>
-      <c r="L21" s="181" t="s">
+      <c r="L21" s="178" t="s">
         <v>1234</v>
       </c>
-      <c r="M21" s="182" t="s">
+      <c r="M21" s="179" t="s">
         <v>19</v>
       </c>
       <c r="N21" s="107"/>
@@ -6506,41 +6527,41 @@
       <c r="AA21" s="116"/>
     </row>
     <row r="22" spans="1:27" s="113" customFormat="1" ht="25" customHeight="1">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="171" t="s">
         <v>1235</v>
       </c>
-      <c r="B22" s="175">
-        <v>1</v>
-      </c>
-      <c r="C22" s="176" t="s">
+      <c r="B22" s="172" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C22" s="173" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="183" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="178" t="s">
+      <c r="D22" s="180" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="175" t="s">
         <v>1233</v>
       </c>
-      <c r="F22" s="179" t="s">
+      <c r="F22" s="176" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="179">
+      <c r="G22" s="176">
         <v>30</v>
       </c>
-      <c r="H22" s="180">
+      <c r="H22" s="177">
         <v>5</v>
       </c>
-      <c r="I22" s="180" t="s">
+      <c r="I22" s="177" t="s">
         <v>96</v>
       </c>
-      <c r="J22" s="180">
+      <c r="J22" s="177">
         <v>2</v>
       </c>
       <c r="K22" s="107"/>
-      <c r="L22" s="181" t="s">
+      <c r="L22" s="178" t="s">
         <v>1234</v>
       </c>
-      <c r="M22" s="184" t="s">
+      <c r="M22" s="181" t="s">
         <v>19</v>
       </c>
       <c r="N22" s="107"/>
@@ -21083,7 +21104,7 @@
       <c r="Z404" s="151"/>
       <c r="AA404" s="151"/>
     </row>
-    <row r="405" spans="1:27" ht="14">
+    <row r="405" spans="1:27" ht="15">
       <c r="A405" s="166" t="s">
         <v>3</v>
       </c>
@@ -21107,7 +21128,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Specify in the comments collumn if DSD sample!" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Index!$G$1:$G$3</xm:f>
@@ -21154,25 +21175,7 @@
           <x14:formula1>
             <xm:f>[1604.5.rml.xlsx]Sheet2!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>M21:M22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{40C6B01E-5119-8E4E-B1C7-7C0AC8FC48A4}">
-          <x14:formula1>
-            <xm:f>[1604.5.rml.xlsx]Sheet2!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J21:J22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7A0121D8-A4B1-CE49-9DAA-97E23CA8B236}">
-          <x14:formula1>
-            <xm:f>[1604.5.rml.xlsx]Sheet2!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>F21:F22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C8FE2404-9766-6041-AC2E-1D82DC68C347}">
-          <x14:formula1>
-            <xm:f>[1604.5.rml.xlsx]Sheet2!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C21:C22</xm:sqref>
+          <xm:sqref>M21:M22 C21:C22 F21:F22 J21:J22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A9F7F2AD-B334-F149-B068-FD9A7471359F}">
           <x14:formula1>
@@ -21199,7 +21202,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="16">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -24029,7 +24032,7 @@
     <col min="11" max="11" width="45.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="32">
+    <row r="1" spans="1:11" ht="34">
       <c r="A1" s="58" t="s">
         <v>109</v>
       </c>

</xml_diff>